<commit_message>
Modified Content and added few features
Anshuman
</commit_message>
<xml_diff>
--- a/IDEA.xlsx
+++ b/IDEA.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t>Front End</t>
   </si>
@@ -293,65 +293,68 @@
     <t>Visitor Tracking using Scan Photo Instantly</t>
   </si>
   <si>
-    <t>Security  - Backup live data Captured by installed camera
+    <t>Event Management</t>
+  </si>
+  <si>
+    <t>Taxi Cab booking</t>
+  </si>
+  <si>
+    <t>Travel Ticketing service</t>
+  </si>
+  <si>
+    <t>Educational Information Center</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>App Creation (Android, Windows)</t>
+  </si>
+  <si>
+    <t>Resume Management of Individual and publish to find opertunities within/outside society</t>
+  </si>
+  <si>
+    <t>Integratin with FF/Twitter/LinkedIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real time Interaction system </t>
+  </si>
+  <si>
+    <t>ZopIm</t>
+  </si>
+  <si>
+    <t>Remote connetion facilities and tracking for help</t>
+  </si>
+  <si>
+    <t>team viewer tool</t>
+  </si>
+  <si>
+    <t>Miss Call facility management and help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic Invoices generation after making Maintenance Collections </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reconsilation of the payment details automatically (instantly, daily, weekly and monthly) </t>
+  </si>
+  <si>
+    <t>Feedback Forms</t>
+  </si>
+  <si>
+    <t>Organize a Party (tool)</t>
+  </si>
+  <si>
+    <t>SEO Implementation</t>
+  </si>
+  <si>
+    <t>Birthday Notification and customization for the Individual</t>
+  </si>
+  <si>
+    <t>Security  - Backup live data Captured by installed CCTV camera
 1) Weekly, Monthly, Half Yearly, Yearly packages</t>
   </si>
   <si>
-    <t>Event Management</t>
-  </si>
-  <si>
-    <t>Taxi Cab booking</t>
-  </si>
-  <si>
-    <t>Travel Ticketing service</t>
-  </si>
-  <si>
-    <t>Educational Information Center</t>
-  </si>
-  <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>App Creation (Android, Windows)</t>
-  </si>
-  <si>
-    <t>Resume Management of Individual and publish to find opertunities within/outside society</t>
-  </si>
-  <si>
-    <t>Integratin with FF/Twitter/LinkedIn</t>
-  </si>
-  <si>
-    <t>Birthday Notification and customization of the Individual Society</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Real time Interaction system </t>
-  </si>
-  <si>
-    <t>ZopIm</t>
-  </si>
-  <si>
-    <t>Remote connetion facilities and tracking for help</t>
-  </si>
-  <si>
-    <t>team viewer tool</t>
-  </si>
-  <si>
-    <t>Miss Call facility management and help</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automatic Invoices generation after making Maintenance Collections </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconsilation of the payment details automatically (instantly, daily, weekly and monthly) </t>
-  </si>
-  <si>
-    <t>Feedback Forms</t>
-  </si>
-  <si>
-    <t>Organize a Party (tool)</t>
-  </si>
-  <si>
-    <t>SEO Implementation</t>
+    <t>Automatic Lighting Management Service - Embeded Implementation</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -549,11 +552,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -858,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H87"/>
+  <dimension ref="A2:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,430 +910,589 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="18" t="s">
         <v>25</v>
       </c>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="15" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14">
+      <c r="A6" s="17">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="18" t="s">
         <v>28</v>
       </c>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="15" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18" t="s">
         <v>35</v>
       </c>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18" t="s">
         <v>36</v>
       </c>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
+      <c r="A11" s="17">
         <v>3</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14">
+      <c r="A14" s="17">
         <v>4</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="18" t="s">
         <v>34</v>
       </c>
+      <c r="C14" s="19"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="C20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
         <v>5</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="15" t="s">
+      <c r="C21" s="19"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="15" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="15" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="15" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19" t="s">
         <v>42</v>
       </c>
       <c r="D26" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="15" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19" t="s">
         <v>44</v>
       </c>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="17"/>
+      <c r="B28" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C28" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="15" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="17"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="17"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="17"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="17"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="17"/>
+      <c r="B44" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="17"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="17"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="17"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="17"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="17"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="17"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="17"/>
+      <c r="B58" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="17"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="17"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="17"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="17"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="17"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="17"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="17"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="17"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="17"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="17"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="17"/>
+      <c r="B69" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="17"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="17"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="17"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="21" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="17"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="17"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="21" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C37" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C39" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C40" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C41" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C44" s="15" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="17"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="17"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A77" s="17"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="17"/>
+      <c r="B78" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" s="19"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="17"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="17"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="17"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="21" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C48" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C50" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D50" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C51" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C54" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C55" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C58" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C59" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C60" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C61" s="15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C64" s="15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C65" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C66" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C67" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C68" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C69" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C70" s="15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C71" s="15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C72" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="C73" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>86</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C76" s="15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C77" s="15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C78" s="19" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C79" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C80" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="C83" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C86" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="C87" s="19" t="s">
-        <v>100</v>
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="17"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="21" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>